<commit_message>
📝 Updating comments and test plan
</commit_message>
<xml_diff>
--- a/Plan de test P5.xlsx
+++ b/Plan de test P5.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefan/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefan/Desktop/Formation Web Dev/Projet 5/Projet Orinoco/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6A0DA9-B9F4-3E4E-84D2-E058AFE02261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03502CE-CCFB-A04B-B90D-441C0B57EF66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,18 +49,12 @@
     <t>main.js</t>
   </si>
   <si>
-    <t>Une fois l'API appelée cette fonction doit permettre de nous afficher le ou les articles disponibles sur notre page web, à partir d'une structure établie</t>
-  </si>
-  <si>
     <t>56 à 121</t>
   </si>
   <si>
     <t>displayArticle</t>
   </si>
   <si>
-    <t>Une fois l'API appelée cette fonction doit permettre de nous afficher le descriptif d'un article sur notre page web, à partir d'une structure établie</t>
-  </si>
-  <si>
     <t>scripts.js</t>
   </si>
   <si>
@@ -73,9 +67,6 @@
     <t>Le nombre d'articles présents dans le panier doit s'afficher dans une bulle située en haut à droite du header</t>
   </si>
   <si>
-    <t>Rajouter ou supprimer un article du panier, le widget dépendant du localStorage, il se met à jour automatiquement</t>
-  </si>
-  <si>
     <t>Si le localSotrage est mal renseigné, ou que la fonction n'est pas appelée au bon endroit le widget ne s'affichera pas</t>
   </si>
   <si>
@@ -203,6 +194,15 @@
   </si>
   <si>
     <t>En finalisant la commande et en vérifiant bien qu'un ID aléatoire s'affiche bien (faire plusieures commandes)</t>
+  </si>
+  <si>
+    <t>Une fois l'API que nous a retourné son data cette fonction doit permettre de nous afficher le descriptif d'un article sur notre page web, à partir d'une structure établie</t>
+  </si>
+  <si>
+    <t>Une fois que l'API nous a retourné son data cette fonction doit permettre de nous afficher le ou les articles disponibles sur notre page web, à partir d'une structure établie</t>
+  </si>
+  <si>
+    <t>Rajouter ou supprimer un article du panier, le widget est dépendant du localStorage, il se met à jour automatiquement</t>
   </si>
 </sst>
 </file>
@@ -527,7 +527,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -592,13 +592,13 @@
         <v>6</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="83" customHeight="1" x14ac:dyDescent="0.15">
@@ -606,179 +606,179 @@
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="D3" s="7" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="D4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="E4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="E6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="F6" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="E7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="F7" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="E11" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="F11" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>